<commit_message>
Add `task-4` in `game-theory`
</commit_message>
<xml_diff>
--- a/3-course-6-semester/game-theory/Бронников Егор ПМ-1901 - minmax f(x,y).xlsx
+++ b/3-course-6-semester/game-theory/Бронников Егор ПМ-1901 - minmax f(x,y).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\egor\github\university\3-course-6-semester\game-theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7F4044-3CA5-4CF1-91A2-0B5CC464EAA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F37D27-74C1-4A7A-8F87-26D6D830914E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C475A2DF-953A-4926-B4CF-8AED05C01FF6}"/>
   </bookViews>
@@ -505,6 +505,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -515,15 +524,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4065,7 +4065,7 @@
   <dimension ref="A1:DA122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB11" sqref="AB11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4116,10 +4116,10 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="5">
         <v>0.01</v>
       </c>
@@ -4130,46 +4130,46 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="37">
+      <c r="B9" s="34"/>
+      <c r="C9" s="33">
         <f>MAX(DA19:DA119)</f>
         <v>9</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="35">
+      <c r="G9" s="37"/>
+      <c r="H9" s="31">
         <f>INDEX(A19:A119,MATCH(C9,DA19:DA119,0))</f>
         <v>-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="37">
+      <c r="B10" s="34"/>
+      <c r="C10" s="33">
         <f>MIN(C122:CY122)</f>
         <v>9</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="36">
+      <c r="G10" s="37"/>
+      <c r="H10" s="32">
         <f>INDEX(C17:CY17,MATCH(C10,C122:CY122,0))</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="31"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="30" t="str">
         <f>IF(C9=C10,"есть","нет")</f>
         <v>есть</v>

</xml_diff>